<commit_message>
Post Job Excel Data
</commit_message>
<xml_diff>
--- a/slingshot/TestData/InputData.xlsx
+++ b/slingshot/TestData/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15120" windowHeight="1920" tabRatio="871" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15120" windowHeight="1920" tabRatio="871" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Failure" sheetId="10" r:id="rId1"/>
@@ -12,31 +12,32 @@
     <sheet name="ChangePrivilageEmail_Success" sheetId="26" r:id="rId3"/>
     <sheet name="ChangePrivilages_Success" sheetId="27" r:id="rId4"/>
     <sheet name="ChangePrivlageSubAdmin_Success" sheetId="29" r:id="rId5"/>
-    <sheet name="ChangePrivilage2Trainer_Success" sheetId="37" r:id="rId6"/>
-    <sheet name="Organisation_Reg_Failure" sheetId="8" r:id="rId7"/>
-    <sheet name="ChangePassword_Failure" sheetId="11" r:id="rId8"/>
-    <sheet name="ChangePassword_Success" sheetId="12" r:id="rId9"/>
-    <sheet name="PodSearch_Success" sheetId="13" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId11"/>
-    <sheet name="LoginAsAdmin_Success" sheetId="14" r:id="rId12"/>
-    <sheet name="IndividualRegister_Failure" sheetId="15" r:id="rId13"/>
-    <sheet name="ForgotPassword_Failure" sheetId="16" r:id="rId14"/>
-    <sheet name="ForgotPassword_Success" sheetId="17" r:id="rId15"/>
-    <sheet name="AddAdmin_Success" sheetId="18" r:id="rId16"/>
-    <sheet name="AddTrainerAdmin_Success" sheetId="23" r:id="rId17"/>
-    <sheet name="AddJobAdmin_Success" sheetId="24" r:id="rId18"/>
-    <sheet name="AddSubAdmin_Success" sheetId="25" r:id="rId19"/>
-    <sheet name="AnotherAdminErrorMsg_Success" sheetId="22" r:id="rId20"/>
-    <sheet name="AddAdmin_Failure" sheetId="19" r:id="rId21"/>
-    <sheet name="LoginAsRemovedAdmin_Success" sheetId="20" r:id="rId22"/>
-    <sheet name="AddAnotherAdmin_Success" sheetId="21" r:id="rId23"/>
+    <sheet name="PostJob_Failure" sheetId="38" r:id="rId6"/>
+    <sheet name="ChangePrivilage2Trainer_Success" sheetId="37" r:id="rId7"/>
+    <sheet name="Organisation_Reg_Failure" sheetId="8" r:id="rId8"/>
+    <sheet name="ChangePassword_Failure" sheetId="11" r:id="rId9"/>
+    <sheet name="ChangePassword_Success" sheetId="12" r:id="rId10"/>
+    <sheet name="PodSearch_Success" sheetId="13" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId12"/>
+    <sheet name="LoginAsAdmin_Success" sheetId="14" r:id="rId13"/>
+    <sheet name="IndividualRegister_Failure" sheetId="15" r:id="rId14"/>
+    <sheet name="ForgotPassword_Failure" sheetId="16" r:id="rId15"/>
+    <sheet name="ForgotPassword_Success" sheetId="17" r:id="rId16"/>
+    <sheet name="AddAdmin_Success" sheetId="18" r:id="rId17"/>
+    <sheet name="AddTrainerAdmin_Success" sheetId="23" r:id="rId18"/>
+    <sheet name="AddJobAdmin_Success" sheetId="24" r:id="rId19"/>
+    <sheet name="AddSubAdmin_Success" sheetId="25" r:id="rId20"/>
+    <sheet name="AnotherAdminErrorMsg_Success" sheetId="22" r:id="rId21"/>
+    <sheet name="AddAdmin_Failure" sheetId="19" r:id="rId22"/>
+    <sheet name="LoginAsRemovedAdmin_Success" sheetId="20" r:id="rId23"/>
+    <sheet name="AddAnotherAdmin_Success" sheetId="21" r:id="rId24"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="233">
   <si>
     <t>Expected Messages</t>
   </si>
@@ -465,13 +466,283 @@
   </si>
   <si>
     <t>rohit.kuma@test.com</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>No of Positions</t>
+  </si>
+  <si>
+    <t>Minimum Age</t>
+  </si>
+  <si>
+    <t>Maximum Age</t>
+  </si>
+  <si>
+    <t>Minimum Experience</t>
+  </si>
+  <si>
+    <t>Maximum Experience</t>
+  </si>
+  <si>
+    <t>Minimum Salary</t>
+  </si>
+  <si>
+    <t>Maximum Salary</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Job Type</t>
+  </si>
+  <si>
+    <t>Job Last Date</t>
+  </si>
+  <si>
+    <t>Job Posting Date</t>
+  </si>
+  <si>
+    <t>Job Expiry Date</t>
+  </si>
+  <si>
+    <t>Education Qualification</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Preferred Certificates</t>
+  </si>
+  <si>
+    <t>Job Description</t>
+  </si>
+  <si>
+    <t>Expected Error Messages</t>
+  </si>
+  <si>
+    <t>jobtitle_req</t>
+  </si>
+  <si>
+    <t>jobtitle_req,noofpositions_req,minage_req,maxage_req,minexperience_req,maxexperience_req,minsalary_req,maxsalary_req,industry_req,location_req,jobtype_req,joblastdate_req,jobpostdate_req,jobexpirydate_req,eduqualification_req,skill_req,jobdesc_req</t>
+  </si>
+  <si>
+    <t>System Engineer</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>350000</t>
+  </si>
+  <si>
+    <t>200000</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Hyderabad Telangana, India</t>
+  </si>
+  <si>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>B.E</t>
+  </si>
+  <si>
+    <t>Air conditioning fundamentals</t>
+  </si>
+  <si>
+    <t>Java Certified</t>
+  </si>
+  <si>
+    <t>Common Job Responsibilities for a Systems Engineer Position: Coordinatesystem development tasks to include design, integration and formal testing. Oversees all transitions into production. Develop and complete actions in systemspecifications, technical and logistical requirements and other disciplines.</t>
+  </si>
+  <si>
+    <t>noofpositions_req</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hadoop Architect </t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>minage_req</t>
+  </si>
+  <si>
+    <t>maxage_req</t>
+  </si>
+  <si>
+    <t>minexperience_req</t>
+  </si>
+  <si>
+    <t>maxexperience_req</t>
+  </si>
+  <si>
+    <t>minsalary_req</t>
+  </si>
+  <si>
+    <t>maxsalary_req</t>
+  </si>
+  <si>
+    <t>industry_req</t>
+  </si>
+  <si>
+    <t>location_req</t>
+  </si>
+  <si>
+    <t>jobtype_req</t>
+  </si>
+  <si>
+    <t>joblastdate_req</t>
+  </si>
+  <si>
+    <t>jobpostdate_req</t>
+  </si>
+  <si>
+    <t>jobexpirydate_req</t>
+  </si>
+  <si>
+    <t>eduqualification_req</t>
+  </si>
+  <si>
+    <t>skill_req</t>
+  </si>
+  <si>
+    <t>jobdesc_req</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>minAgeGreaterMax</t>
+  </si>
+  <si>
+    <t>minExpGreaterMax</t>
+  </si>
+  <si>
+    <t>minSalGreaterMax</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>lastAfterPosting_date,jobpostingBeforeLast_date</t>
+  </si>
+  <si>
+    <t>lastAfterExpiry_date,postingBeforeExpiry_date,expiryAfterPosting_date,expiryAfterLast_date</t>
+  </si>
+  <si>
+    <t>lastAfterPosting_date,lastAfterExpiry_date,postingBeforeExpiry_date,jobpostingBeforeLast_date,expiryAfterPosting_date,expiryAfterLast_date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -649,8 +920,15 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="29">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,6 +1073,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1006,7 +1290,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1084,6 +1368,16 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="58">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1145,19 +1439,7 @@
     <cellStyle name="Total 2" xfId="55"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="492">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="491">
     <dxf>
       <font>
         <sz val="11"/>
@@ -6885,13 +7167,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C2">
-    <cfRule type="duplicateValues" dxfId="491" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="490" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:C3">
-    <cfRule type="duplicateValues" dxfId="490" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="489" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:C4">
-    <cfRule type="duplicateValues" dxfId="489" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="488" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6899,6 +7181,94 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="337" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="336" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="duplicateValues" dxfId="335" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="duplicateValues" dxfId="334" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="333" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="332" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="duplicateValues" dxfId="331" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="duplicateValues" dxfId="330" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -6940,16 +7310,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="330" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="329" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="329" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="328" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
@@ -7362,403 +7732,403 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="duplicateValues" dxfId="328" priority="131"/>
+    <cfRule type="duplicateValues" dxfId="327" priority="131"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:D1">
-    <cfRule type="duplicateValues" dxfId="327" priority="130"/>
+    <cfRule type="duplicateValues" dxfId="326" priority="130"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2 F5">
-    <cfRule type="duplicateValues" dxfId="326" priority="129"/>
+    <cfRule type="duplicateValues" dxfId="325" priority="129"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M7">
-    <cfRule type="duplicateValues" dxfId="325" priority="128"/>
+    <cfRule type="duplicateValues" dxfId="324" priority="128"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:K1">
-    <cfRule type="duplicateValues" dxfId="324" priority="127"/>
+    <cfRule type="duplicateValues" dxfId="323" priority="127"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="duplicateValues" dxfId="323" priority="126"/>
+    <cfRule type="duplicateValues" dxfId="322" priority="126"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="322" priority="125"/>
+    <cfRule type="duplicateValues" dxfId="321" priority="125"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="321" priority="124"/>
+    <cfRule type="duplicateValues" dxfId="320" priority="124"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:K2">
-    <cfRule type="duplicateValues" dxfId="320" priority="123"/>
+    <cfRule type="duplicateValues" dxfId="319" priority="123"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="duplicateValues" dxfId="319" priority="122"/>
+    <cfRule type="duplicateValues" dxfId="318" priority="122"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="318" priority="121"/>
+    <cfRule type="duplicateValues" dxfId="317" priority="121"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="duplicateValues" dxfId="317" priority="120"/>
+    <cfRule type="duplicateValues" dxfId="316" priority="120"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="duplicateValues" dxfId="316" priority="119"/>
+    <cfRule type="duplicateValues" dxfId="315" priority="119"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:K3">
-    <cfRule type="duplicateValues" dxfId="315" priority="118"/>
+    <cfRule type="duplicateValues" dxfId="314" priority="118"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="duplicateValues" dxfId="314" priority="117"/>
+    <cfRule type="duplicateValues" dxfId="313" priority="117"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="duplicateValues" dxfId="313" priority="116"/>
+    <cfRule type="duplicateValues" dxfId="312" priority="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:K4">
-    <cfRule type="duplicateValues" dxfId="312" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="311" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="duplicateValues" dxfId="311" priority="114"/>
+    <cfRule type="duplicateValues" dxfId="310" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="duplicateValues" dxfId="310" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="309" priority="113"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:H5">
-    <cfRule type="duplicateValues" dxfId="309" priority="112"/>
+    <cfRule type="duplicateValues" dxfId="308" priority="112"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:K5">
-    <cfRule type="duplicateValues" dxfId="308" priority="111"/>
+    <cfRule type="duplicateValues" dxfId="307" priority="111"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="duplicateValues" dxfId="307" priority="110"/>
+    <cfRule type="duplicateValues" dxfId="306" priority="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="duplicateValues" dxfId="306" priority="109"/>
+    <cfRule type="duplicateValues" dxfId="305" priority="109"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="duplicateValues" dxfId="305" priority="108"/>
+    <cfRule type="duplicateValues" dxfId="304" priority="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:K6">
-    <cfRule type="duplicateValues" dxfId="304" priority="107"/>
+    <cfRule type="duplicateValues" dxfId="303" priority="107"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="duplicateValues" dxfId="303" priority="106"/>
+    <cfRule type="duplicateValues" dxfId="302" priority="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:K7">
-    <cfRule type="duplicateValues" dxfId="302" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="301" priority="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="duplicateValues" dxfId="301" priority="104"/>
+    <cfRule type="duplicateValues" dxfId="300" priority="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="duplicateValues" dxfId="300" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="299" priority="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="duplicateValues" dxfId="299" priority="102"/>
+    <cfRule type="duplicateValues" dxfId="298" priority="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="duplicateValues" dxfId="298" priority="101"/>
+    <cfRule type="duplicateValues" dxfId="297" priority="101"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8">
-    <cfRule type="duplicateValues" dxfId="297" priority="100"/>
+    <cfRule type="duplicateValues" dxfId="296" priority="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="296" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="295" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="295" priority="98"/>
+    <cfRule type="duplicateValues" dxfId="294" priority="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="duplicateValues" dxfId="294" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="293" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="duplicateValues" dxfId="293" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="292" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="292" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="291" priority="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="291" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="290" priority="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="duplicateValues" dxfId="290" priority="93"/>
+    <cfRule type="duplicateValues" dxfId="289" priority="93"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="duplicateValues" dxfId="289" priority="92"/>
+    <cfRule type="duplicateValues" dxfId="288" priority="92"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="288" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="287" priority="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="287" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="286" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="duplicateValues" dxfId="286" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="285" priority="89"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="duplicateValues" dxfId="285" priority="88"/>
+    <cfRule type="duplicateValues" dxfId="284" priority="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="duplicateValues" dxfId="284" priority="87"/>
+    <cfRule type="duplicateValues" dxfId="283" priority="87"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="duplicateValues" dxfId="283" priority="86"/>
+    <cfRule type="duplicateValues" dxfId="282" priority="86"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="duplicateValues" dxfId="282" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="281" priority="85"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
-    <cfRule type="duplicateValues" dxfId="281" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="280" priority="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="duplicateValues" dxfId="280" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="279" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="279" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="278" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="278" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="277" priority="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="duplicateValues" dxfId="277" priority="80"/>
+    <cfRule type="duplicateValues" dxfId="276" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="duplicateValues" dxfId="276" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="275" priority="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="duplicateValues" dxfId="275" priority="78"/>
+    <cfRule type="duplicateValues" dxfId="274" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="duplicateValues" dxfId="274" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="273" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="duplicateValues" dxfId="273" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="272" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="duplicateValues" dxfId="272" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="271" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="271" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="270" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="270" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="269" priority="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="269" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="268" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="268" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="267" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="267" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="266" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="266" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="265" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="265" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="264" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="264" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="263" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="duplicateValues" dxfId="263" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="262" priority="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="duplicateValues" dxfId="262" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="261" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="261" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="260" priority="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="duplicateValues" dxfId="260" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="259" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="duplicateValues" dxfId="259" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="258" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="duplicateValues" dxfId="258" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="257" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="duplicateValues" dxfId="257" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="256" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="duplicateValues" dxfId="256" priority="60"/>
+    <cfRule type="duplicateValues" dxfId="255" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="duplicateValues" dxfId="255" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="254" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="duplicateValues" dxfId="254" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="253" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="duplicateValues" dxfId="253" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="252" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="duplicateValues" dxfId="252" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="251" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="duplicateValues" dxfId="251" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="250" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="250" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="249" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="duplicateValues" dxfId="249" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="248" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="duplicateValues" dxfId="248" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="247" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="duplicateValues" dxfId="247" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="246" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="duplicateValues" dxfId="246" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="245" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="duplicateValues" dxfId="245" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="244" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="duplicateValues" dxfId="244" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="243" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="duplicateValues" dxfId="243" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="242" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="duplicateValues" dxfId="242" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="241" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1">
-    <cfRule type="duplicateValues" dxfId="241" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="240" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="duplicateValues" dxfId="240" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="239" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="239" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="238" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="duplicateValues" dxfId="238" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="237" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="duplicateValues" dxfId="237" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="236" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="duplicateValues" dxfId="236" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="235" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="duplicateValues" dxfId="235" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="234" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="duplicateValues" dxfId="234" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="233" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="duplicateValues" dxfId="233" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="232" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="duplicateValues" dxfId="232" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="231" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="duplicateValues" dxfId="231" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="230" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="duplicateValues" dxfId="230" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="229" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="duplicateValues" dxfId="229" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="228" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="duplicateValues" dxfId="228" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="227" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="duplicateValues" dxfId="227" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="226" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="duplicateValues" dxfId="226" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="225" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="duplicateValues" dxfId="225" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="224" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="duplicateValues" dxfId="224" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="223" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="duplicateValues" dxfId="223" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="222" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="duplicateValues" dxfId="222" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="221" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="duplicateValues" dxfId="221" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="220" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="duplicateValues" dxfId="220" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="219" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="duplicateValues" dxfId="219" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="218" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="duplicateValues" dxfId="218" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="217" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="duplicateValues" dxfId="217" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="216" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="duplicateValues" dxfId="216" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="215" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="duplicateValues" dxfId="215" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="214" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="duplicateValues" dxfId="214" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="213" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="duplicateValues" dxfId="213" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="212" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="212" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="211" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="duplicateValues" dxfId="211" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="210" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="duplicateValues" dxfId="210" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="209" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="209" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="208" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="duplicateValues" dxfId="208" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="207" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="duplicateValues" dxfId="207" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="206" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="duplicateValues" dxfId="206" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="205" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="205" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="204" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="204" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="203" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="duplicateValues" dxfId="203" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="202" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="202" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="201" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="duplicateValues" dxfId="201" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="200" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="duplicateValues" dxfId="200" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="199" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="199" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="198" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="duplicateValues" dxfId="198" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="197" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -7796,14 +8166,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C2">
-    <cfRule type="duplicateValues" dxfId="197" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="196" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
@@ -8349,365 +8719,365 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H10">
-    <cfRule type="duplicateValues" dxfId="196" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="195" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="duplicateValues" dxfId="195" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="194" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4">
-    <cfRule type="duplicateValues" dxfId="194" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="193" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="duplicateValues" dxfId="193" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="192" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="duplicateValues" dxfId="192" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="191" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="duplicateValues" dxfId="191" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="190" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="duplicateValues" dxfId="190" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="189" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="duplicateValues" dxfId="189" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="188" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="duplicateValues" dxfId="188" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="187" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5">
-    <cfRule type="duplicateValues" dxfId="187" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="186" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" dxfId="186" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="185" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="duplicateValues" dxfId="185" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="184" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="duplicateValues" dxfId="184" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="183" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="duplicateValues" dxfId="183" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="182" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="duplicateValues" dxfId="182" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="181" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="duplicateValues" dxfId="181" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="180" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="180" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="179" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="duplicateValues" dxfId="179" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="178" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="177" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="duplicateValues" dxfId="177" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="176" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="176" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="duplicateValues" dxfId="175" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="174" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:J6">
-    <cfRule type="duplicateValues" dxfId="174" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="duplicateValues" dxfId="173" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="duplicateValues" dxfId="172" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="duplicateValues" dxfId="171" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="duplicateValues" dxfId="170" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="duplicateValues" dxfId="169" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="168" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="duplicateValues" dxfId="167" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:J7">
-    <cfRule type="duplicateValues" dxfId="166" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="duplicateValues" dxfId="165" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="duplicateValues" dxfId="164" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="duplicateValues" dxfId="163" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="duplicateValues" dxfId="162" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="duplicateValues" dxfId="161" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="160" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="duplicateValues" dxfId="159" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:J8">
-    <cfRule type="duplicateValues" dxfId="158" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="duplicateValues" dxfId="157" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="duplicateValues" dxfId="156" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="duplicateValues" dxfId="155" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="duplicateValues" dxfId="154" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="153" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="duplicateValues" dxfId="152" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:J9">
-    <cfRule type="duplicateValues" dxfId="151" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="duplicateValues" dxfId="150" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="duplicateValues" dxfId="149" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="duplicateValues" dxfId="148" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="duplicateValues" dxfId="147" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="146" priority="60"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="145" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:J10">
-    <cfRule type="duplicateValues" dxfId="144" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="duplicateValues" dxfId="143" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="duplicateValues" dxfId="142" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="duplicateValues" dxfId="141" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="140" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="139" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:J11">
-    <cfRule type="duplicateValues" dxfId="138" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="duplicateValues" dxfId="137" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="duplicateValues" dxfId="136" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="135" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="duplicateValues" dxfId="134" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="133" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="duplicateValues" dxfId="132" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:J12">
-    <cfRule type="duplicateValues" dxfId="131" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="duplicateValues" dxfId="130" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="duplicateValues" dxfId="129" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="128" priority="78"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="duplicateValues" dxfId="127" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="duplicateValues" dxfId="126" priority="80"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="duplicateValues" dxfId="125" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="duplicateValues" dxfId="124" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="duplicateValues" dxfId="123" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="duplicateValues" dxfId="122" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="duplicateValues" dxfId="121" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="85"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="duplicateValues" dxfId="120" priority="86"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="86"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="119" priority="87"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="87"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="duplicateValues" dxfId="118" priority="88"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="duplicateValues" dxfId="117" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="89"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="duplicateValues" dxfId="116" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="duplicateValues" dxfId="115" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="duplicateValues" dxfId="114" priority="92"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="92"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="duplicateValues" dxfId="113" priority="93"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="93"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="duplicateValues" dxfId="112" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="duplicateValues" dxfId="111" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="duplicateValues" dxfId="110" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" dxfId="109" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="108" priority="98"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="duplicateValues" dxfId="107" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="duplicateValues" dxfId="106" priority="100"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="duplicateValues" dxfId="105" priority="101"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="101"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="104" priority="102"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="duplicateValues" dxfId="103" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="duplicateValues" dxfId="102" priority="104"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="duplicateValues" dxfId="101" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="duplicateValues" dxfId="100" priority="106"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="duplicateValues" dxfId="99" priority="107"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="107"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="duplicateValues" dxfId="98" priority="108"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="duplicateValues" dxfId="97" priority="109"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="109"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="duplicateValues" dxfId="96" priority="110"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="duplicateValues" dxfId="95" priority="111"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="111"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="duplicateValues" dxfId="94" priority="112"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="112"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="duplicateValues" dxfId="93" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="113"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="duplicateValues" dxfId="92" priority="114"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="duplicateValues" dxfId="91" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="duplicateValues" dxfId="90" priority="116"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="duplicateValues" dxfId="89" priority="117"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="117"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="duplicateValues" dxfId="88" priority="118"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="118"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="duplicateValues" dxfId="87" priority="119"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="119"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="duplicateValues" dxfId="86" priority="120"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="120"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B3">
-    <cfRule type="duplicateValues" dxfId="85" priority="121"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="121"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:J3">
-    <cfRule type="duplicateValues" dxfId="84" priority="122"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="122"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="duplicateValues" dxfId="83" priority="123"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="123"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="duplicateValues" dxfId="82" priority="124"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="124"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="duplicateValues" dxfId="81" priority="125"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="125"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="duplicateValues" dxfId="80" priority="126"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="126"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="duplicateValues" dxfId="79" priority="127"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="127"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -8806,7 +9176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -8873,7 +9243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AKW2"/>
   <sheetViews>
@@ -8962,23 +9332,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="duplicateValues" dxfId="78" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="duplicateValues" dxfId="77" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="76" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="duplicateValues" dxfId="75" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -9066,25 +9436,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="duplicateValues" dxfId="74" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="duplicateValues" dxfId="73" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="duplicateValues" dxfId="72" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="71" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="duplicateValues" dxfId="70" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -9173,121 +9543,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="duplicateValues" dxfId="67" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="66" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="duplicateValues" dxfId="65" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="9" width="9.140625" style="2"/>
-    <col min="10" max="10" width="17.42578125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="J1" s="31" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:B2">
-    <cfRule type="duplicateValues" dxfId="64" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
-    <cfRule type="duplicateValues" dxfId="63" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="duplicateValues" dxfId="62" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="61" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="duplicateValues" dxfId="60" priority="5"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -9329,7 +9600,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C2">
-    <cfRule type="duplicateValues" dxfId="488" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="487" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9337,6 +9608,105 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="17.42578125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:B2">
+    <cfRule type="duplicateValues" dxfId="63" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2">
+    <cfRule type="duplicateValues" dxfId="62" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="duplicateValues" dxfId="61" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="duplicateValues" dxfId="60" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="duplicateValues" dxfId="59" priority="5"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -9369,7 +9739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -9442,7 +9812,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>82</v>
@@ -9472,7 +9842,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>87</v>
       </c>
@@ -9502,7 +9872,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>87</v>
       </c>
@@ -9566,7 +9936,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>87</v>
       </c>
@@ -9596,7 +9966,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>87</v>
       </c>
@@ -9692,173 +10062,173 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:B3">
-    <cfRule type="duplicateValues" dxfId="59" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="duplicateValues" dxfId="57" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="duplicateValues" dxfId="55" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:B4">
-    <cfRule type="duplicateValues" dxfId="54" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="duplicateValues" dxfId="53" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="duplicateValues" dxfId="52" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="duplicateValues" dxfId="51" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="duplicateValues" dxfId="50" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="49" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="duplicateValues" dxfId="48" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="duplicateValues" dxfId="47" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="duplicateValues" dxfId="46" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="duplicateValues" dxfId="45" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="44" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="duplicateValues" dxfId="43" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="duplicateValues" dxfId="42" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="duplicateValues" dxfId="41" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="duplicateValues" dxfId="40" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="39" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="duplicateValues" dxfId="38" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="duplicateValues" dxfId="37" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="duplicateValues" dxfId="36" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="duplicateValues" dxfId="35" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="34" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="duplicateValues" dxfId="33" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="duplicateValues" dxfId="32" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="duplicateValues" dxfId="31" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="duplicateValues" dxfId="30" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="29" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="duplicateValues" dxfId="28" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="duplicateValues" dxfId="27" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="duplicateValues" dxfId="26" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="duplicateValues" dxfId="25" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="duplicateValues" dxfId="24" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="23" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="22" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="21" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="20" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="19" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="18" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" dxfId="17" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="duplicateValues" dxfId="16" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="duplicateValues" dxfId="15" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="14" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="13" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="duplicateValues" dxfId="12" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="duplicateValues" dxfId="11" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="duplicateValues" dxfId="10" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2">
-    <cfRule type="duplicateValues" dxfId="9" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="duplicateValues" dxfId="8" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="duplicateValues" dxfId="7" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="duplicateValues" dxfId="6" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="54"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -9891,7 +10261,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:C2">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -9902,7 +10272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -9991,7 +10361,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
@@ -10093,7 +10463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -10133,6 +10503,1377 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" customWidth="1"/>
+    <col min="15" max="15" width="26.28515625" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="27.85546875" customWidth="1"/>
+    <col min="18" max="19" width="45.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="P1" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q1" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="R1" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="S1" s="37" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+      <c r="S2" s="38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="B3" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L3" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M3" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N3" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O3" t="s">
+        <v>173</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>175</v>
+      </c>
+      <c r="R3" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I4" t="s">
+        <v>170</v>
+      </c>
+      <c r="J4" t="s">
+        <v>171</v>
+      </c>
+      <c r="K4" t="s">
+        <v>172</v>
+      </c>
+      <c r="L4" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M4" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N4" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O4" t="s">
+        <v>173</v>
+      </c>
+      <c r="P4" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>175</v>
+      </c>
+      <c r="R4" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I5" t="s">
+        <v>170</v>
+      </c>
+      <c r="J5" t="s">
+        <v>171</v>
+      </c>
+      <c r="K5" t="s">
+        <v>172</v>
+      </c>
+      <c r="L5" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M5" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N5" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O5" t="s">
+        <v>173</v>
+      </c>
+      <c r="P5" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>175</v>
+      </c>
+      <c r="R5" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I6" t="s">
+        <v>170</v>
+      </c>
+      <c r="J6" t="s">
+        <v>171</v>
+      </c>
+      <c r="K6" t="s">
+        <v>172</v>
+      </c>
+      <c r="L6" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M6" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N6" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O6" t="s">
+        <v>173</v>
+      </c>
+      <c r="P6" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>175</v>
+      </c>
+      <c r="R6" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" t="s">
+        <v>170</v>
+      </c>
+      <c r="J7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K7" t="s">
+        <v>172</v>
+      </c>
+      <c r="L7" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M7" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N7" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O7" t="s">
+        <v>173</v>
+      </c>
+      <c r="P7" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>175</v>
+      </c>
+      <c r="R7" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J8" t="s">
+        <v>171</v>
+      </c>
+      <c r="K8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L8" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M8" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N8" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O8" t="s">
+        <v>173</v>
+      </c>
+      <c r="P8" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>175</v>
+      </c>
+      <c r="R8" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I9" t="s">
+        <v>170</v>
+      </c>
+      <c r="J9" t="s">
+        <v>171</v>
+      </c>
+      <c r="K9" t="s">
+        <v>172</v>
+      </c>
+      <c r="L9" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M9" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N9" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O9" t="s">
+        <v>173</v>
+      </c>
+      <c r="P9" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>175</v>
+      </c>
+      <c r="R9" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J10" t="s">
+        <v>171</v>
+      </c>
+      <c r="K10" t="s">
+        <v>172</v>
+      </c>
+      <c r="L10" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M10" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N10" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O10" t="s">
+        <v>173</v>
+      </c>
+      <c r="P10" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>175</v>
+      </c>
+      <c r="R10" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="J11" t="s">
+        <v>171</v>
+      </c>
+      <c r="K11" t="s">
+        <v>172</v>
+      </c>
+      <c r="L11" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M11" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N11" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O11" t="s">
+        <v>173</v>
+      </c>
+      <c r="P11" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>175</v>
+      </c>
+      <c r="R11" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I12" t="s">
+        <v>170</v>
+      </c>
+      <c r="K12" t="s">
+        <v>172</v>
+      </c>
+      <c r="L12" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M12" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N12" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O12" t="s">
+        <v>173</v>
+      </c>
+      <c r="P12" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>175</v>
+      </c>
+      <c r="R12" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I13" t="s">
+        <v>170</v>
+      </c>
+      <c r="J13" t="s">
+        <v>171</v>
+      </c>
+      <c r="L13" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M13" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N13" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O13" t="s">
+        <v>173</v>
+      </c>
+      <c r="P13" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>175</v>
+      </c>
+      <c r="R13" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I14" t="s">
+        <v>170</v>
+      </c>
+      <c r="J14" t="s">
+        <v>171</v>
+      </c>
+      <c r="K14" t="s">
+        <v>172</v>
+      </c>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N14" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O14" t="s">
+        <v>173</v>
+      </c>
+      <c r="P14" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>175</v>
+      </c>
+      <c r="R14" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I15" t="s">
+        <v>170</v>
+      </c>
+      <c r="J15" t="s">
+        <v>171</v>
+      </c>
+      <c r="K15" t="s">
+        <v>172</v>
+      </c>
+      <c r="L15" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M15" s="40"/>
+      <c r="N15" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O15" t="s">
+        <v>173</v>
+      </c>
+      <c r="P15" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>175</v>
+      </c>
+      <c r="R15" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J16" t="s">
+        <v>171</v>
+      </c>
+      <c r="K16" t="s">
+        <v>172</v>
+      </c>
+      <c r="L16" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M16" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N16" s="41"/>
+      <c r="O16" t="s">
+        <v>173</v>
+      </c>
+      <c r="P16" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>175</v>
+      </c>
+      <c r="R16" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H17" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" t="s">
+        <v>170</v>
+      </c>
+      <c r="J17" t="s">
+        <v>171</v>
+      </c>
+      <c r="K17" t="s">
+        <v>172</v>
+      </c>
+      <c r="L17" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M17" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N17" s="41">
+        <v>42885</v>
+      </c>
+      <c r="P17" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>175</v>
+      </c>
+      <c r="R17" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H18" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I18" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" t="s">
+        <v>171</v>
+      </c>
+      <c r="K18" t="s">
+        <v>172</v>
+      </c>
+      <c r="L18" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M18" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N18" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O18" t="s">
+        <v>173</v>
+      </c>
+      <c r="P18" s="38"/>
+      <c r="Q18" t="s">
+        <v>175</v>
+      </c>
+      <c r="R18" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H19" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I19" t="s">
+        <v>170</v>
+      </c>
+      <c r="J19" t="s">
+        <v>171</v>
+      </c>
+      <c r="K19" t="s">
+        <v>172</v>
+      </c>
+      <c r="L19" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M19" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N19" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O19" t="s">
+        <v>173</v>
+      </c>
+      <c r="P19" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>175</v>
+      </c>
+      <c r="R19" s="42"/>
+      <c r="S19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F20" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H20" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I20" t="s">
+        <v>170</v>
+      </c>
+      <c r="J20" t="s">
+        <v>171</v>
+      </c>
+      <c r="K20" t="s">
+        <v>172</v>
+      </c>
+      <c r="L20" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M20" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N20" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O20" t="s">
+        <v>173</v>
+      </c>
+      <c r="P20" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>175</v>
+      </c>
+      <c r="R20" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="H21" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="I21" t="s">
+        <v>170</v>
+      </c>
+      <c r="J21" t="s">
+        <v>171</v>
+      </c>
+      <c r="K21" t="s">
+        <v>172</v>
+      </c>
+      <c r="L21" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M21" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N21" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O21" t="s">
+        <v>173</v>
+      </c>
+      <c r="P21" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>175</v>
+      </c>
+      <c r="R21" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="H22" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="I22" t="s">
+        <v>170</v>
+      </c>
+      <c r="J22" t="s">
+        <v>171</v>
+      </c>
+      <c r="K22" t="s">
+        <v>172</v>
+      </c>
+      <c r="L22" s="40">
+        <v>42840</v>
+      </c>
+      <c r="M22" s="40">
+        <v>42832</v>
+      </c>
+      <c r="N22" s="41">
+        <v>42885</v>
+      </c>
+      <c r="O22" t="s">
+        <v>173</v>
+      </c>
+      <c r="P22" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>175</v>
+      </c>
+      <c r="R22" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S22" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="H23" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="I23" t="s">
+        <v>170</v>
+      </c>
+      <c r="J23" t="s">
+        <v>171</v>
+      </c>
+      <c r="K23" t="s">
+        <v>172</v>
+      </c>
+      <c r="L23" s="40">
+        <v>42834</v>
+      </c>
+      <c r="M23" s="40">
+        <v>42834</v>
+      </c>
+      <c r="N23" s="40">
+        <v>42852</v>
+      </c>
+      <c r="O23" t="s">
+        <v>173</v>
+      </c>
+      <c r="P23" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>175</v>
+      </c>
+      <c r="R23" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="H24" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="I24" t="s">
+        <v>170</v>
+      </c>
+      <c r="J24" t="s">
+        <v>171</v>
+      </c>
+      <c r="K24" t="s">
+        <v>172</v>
+      </c>
+      <c r="L24" s="40">
+        <v>42846</v>
+      </c>
+      <c r="M24" s="40">
+        <v>42845</v>
+      </c>
+      <c r="N24" s="40">
+        <v>42836</v>
+      </c>
+      <c r="O24" t="s">
+        <v>173</v>
+      </c>
+      <c r="P24" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>175</v>
+      </c>
+      <c r="R24" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="S24" s="38" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L25" s="40">
+        <v>42875</v>
+      </c>
+      <c r="M25" s="40">
+        <v>42889</v>
+      </c>
+      <c r="N25" s="40">
+        <v>42836</v>
+      </c>
+      <c r="S25" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -10176,12 +11917,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10636,410 +12377,410 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B2">
-    <cfRule type="duplicateValues" dxfId="487" priority="355"/>
+    <cfRule type="duplicateValues" dxfId="486" priority="355"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D2">
-    <cfRule type="duplicateValues" dxfId="486" priority="354"/>
+    <cfRule type="duplicateValues" dxfId="485" priority="354"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F2">
-    <cfRule type="duplicateValues" dxfId="485" priority="353"/>
+    <cfRule type="duplicateValues" dxfId="484" priority="353"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:H2">
-    <cfRule type="duplicateValues" dxfId="484" priority="352"/>
+    <cfRule type="duplicateValues" dxfId="483" priority="352"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2 M2">
-    <cfRule type="duplicateValues" dxfId="483" priority="351"/>
+    <cfRule type="duplicateValues" dxfId="482" priority="351"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:L2">
-    <cfRule type="duplicateValues" dxfId="482" priority="350"/>
+    <cfRule type="duplicateValues" dxfId="481" priority="350"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="duplicateValues" dxfId="481" priority="349"/>
+    <cfRule type="duplicateValues" dxfId="480" priority="349"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="duplicateValues" dxfId="480" priority="347"/>
+    <cfRule type="duplicateValues" dxfId="479" priority="347"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="duplicateValues" dxfId="479" priority="132"/>
+    <cfRule type="duplicateValues" dxfId="478" priority="132"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B3">
-    <cfRule type="duplicateValues" dxfId="478" priority="131"/>
+    <cfRule type="duplicateValues" dxfId="477" priority="131"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:D3">
-    <cfRule type="duplicateValues" dxfId="477" priority="130"/>
+    <cfRule type="duplicateValues" dxfId="476" priority="130"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4 F7">
-    <cfRule type="duplicateValues" dxfId="476" priority="129"/>
+    <cfRule type="duplicateValues" dxfId="475" priority="129"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M9">
-    <cfRule type="duplicateValues" dxfId="475" priority="128"/>
+    <cfRule type="duplicateValues" dxfId="474" priority="128"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:K3">
-    <cfRule type="duplicateValues" dxfId="474" priority="127"/>
+    <cfRule type="duplicateValues" dxfId="473" priority="127"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="duplicateValues" dxfId="473" priority="126"/>
+    <cfRule type="duplicateValues" dxfId="472" priority="126"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="duplicateValues" dxfId="472" priority="125"/>
+    <cfRule type="duplicateValues" dxfId="471" priority="125"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="duplicateValues" dxfId="471" priority="124"/>
+    <cfRule type="duplicateValues" dxfId="470" priority="124"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:K4">
-    <cfRule type="duplicateValues" dxfId="470" priority="123"/>
+    <cfRule type="duplicateValues" dxfId="469" priority="123"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="duplicateValues" dxfId="469" priority="122"/>
+    <cfRule type="duplicateValues" dxfId="468" priority="122"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="duplicateValues" dxfId="468" priority="121"/>
+    <cfRule type="duplicateValues" dxfId="467" priority="121"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="duplicateValues" dxfId="467" priority="120"/>
+    <cfRule type="duplicateValues" dxfId="466" priority="120"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="duplicateValues" dxfId="466" priority="119"/>
+    <cfRule type="duplicateValues" dxfId="465" priority="119"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:K5">
-    <cfRule type="duplicateValues" dxfId="465" priority="118"/>
+    <cfRule type="duplicateValues" dxfId="464" priority="118"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="duplicateValues" dxfId="464" priority="117"/>
+    <cfRule type="duplicateValues" dxfId="463" priority="117"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="duplicateValues" dxfId="463" priority="116"/>
+    <cfRule type="duplicateValues" dxfId="462" priority="116"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:K6">
-    <cfRule type="duplicateValues" dxfId="462" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="461" priority="115"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P6">
-    <cfRule type="duplicateValues" dxfId="461" priority="114"/>
+    <cfRule type="duplicateValues" dxfId="460" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="duplicateValues" dxfId="460" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="459" priority="113"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:H7">
-    <cfRule type="duplicateValues" dxfId="459" priority="112"/>
+    <cfRule type="duplicateValues" dxfId="458" priority="112"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:K7">
-    <cfRule type="duplicateValues" dxfId="458" priority="111"/>
+    <cfRule type="duplicateValues" dxfId="457" priority="111"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="duplicateValues" dxfId="457" priority="110"/>
+    <cfRule type="duplicateValues" dxfId="456" priority="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="duplicateValues" dxfId="456" priority="109"/>
+    <cfRule type="duplicateValues" dxfId="455" priority="109"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="duplicateValues" dxfId="455" priority="108"/>
+    <cfRule type="duplicateValues" dxfId="454" priority="108"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:K8">
-    <cfRule type="duplicateValues" dxfId="454" priority="107"/>
+    <cfRule type="duplicateValues" dxfId="453" priority="107"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8">
-    <cfRule type="duplicateValues" dxfId="453" priority="106"/>
+    <cfRule type="duplicateValues" dxfId="452" priority="106"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:K9">
-    <cfRule type="duplicateValues" dxfId="452" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="451" priority="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9">
-    <cfRule type="duplicateValues" dxfId="451" priority="104"/>
+    <cfRule type="duplicateValues" dxfId="450" priority="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="duplicateValues" dxfId="450" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="449" priority="103"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="duplicateValues" dxfId="449" priority="102"/>
+    <cfRule type="duplicateValues" dxfId="448" priority="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:K10">
-    <cfRule type="duplicateValues" dxfId="448" priority="101"/>
+    <cfRule type="duplicateValues" dxfId="447" priority="101"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10">
-    <cfRule type="duplicateValues" dxfId="447" priority="100"/>
+    <cfRule type="duplicateValues" dxfId="446" priority="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="446" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="445" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="445" priority="98"/>
+    <cfRule type="duplicateValues" dxfId="444" priority="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="duplicateValues" dxfId="444" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="443" priority="97"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="duplicateValues" dxfId="443" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="442" priority="96"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="442" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="441" priority="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="441" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="440" priority="94"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="duplicateValues" dxfId="440" priority="93"/>
+    <cfRule type="duplicateValues" dxfId="439" priority="93"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="duplicateValues" dxfId="439" priority="92"/>
+    <cfRule type="duplicateValues" dxfId="438" priority="92"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="438" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="437" priority="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="437" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="436" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="duplicateValues" dxfId="436" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="435" priority="89"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="duplicateValues" dxfId="435" priority="88"/>
+    <cfRule type="duplicateValues" dxfId="434" priority="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="duplicateValues" dxfId="434" priority="87"/>
+    <cfRule type="duplicateValues" dxfId="433" priority="87"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="duplicateValues" dxfId="433" priority="86"/>
+    <cfRule type="duplicateValues" dxfId="432" priority="86"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="duplicateValues" dxfId="432" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="431" priority="85"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:K11">
-    <cfRule type="duplicateValues" dxfId="431" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="430" priority="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P11">
-    <cfRule type="duplicateValues" dxfId="430" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="429" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="duplicateValues" dxfId="429" priority="82"/>
+    <cfRule type="duplicateValues" dxfId="428" priority="82"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="428" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="427" priority="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="duplicateValues" dxfId="427" priority="80"/>
+    <cfRule type="duplicateValues" dxfId="426" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="duplicateValues" dxfId="426" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="425" priority="79"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="duplicateValues" dxfId="425" priority="78"/>
+    <cfRule type="duplicateValues" dxfId="424" priority="78"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="duplicateValues" dxfId="424" priority="77"/>
+    <cfRule type="duplicateValues" dxfId="423" priority="77"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="duplicateValues" dxfId="423" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="422" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="duplicateValues" dxfId="422" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="421" priority="75"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="421" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="420" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="420" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="419" priority="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="419" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="418" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="418" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="417" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="417" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="416" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="416" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="415" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="415" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="414" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="414" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="413" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="duplicateValues" dxfId="413" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="412" priority="66"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="duplicateValues" dxfId="412" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="411" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="duplicateValues" dxfId="411" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="410" priority="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="duplicateValues" dxfId="410" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="409" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="duplicateValues" dxfId="409" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="408" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="duplicateValues" dxfId="408" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="407" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="duplicateValues" dxfId="407" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="406" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="duplicateValues" dxfId="406" priority="60"/>
+    <cfRule type="duplicateValues" dxfId="405" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="duplicateValues" dxfId="405" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="404" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="duplicateValues" dxfId="404" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="403" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="duplicateValues" dxfId="403" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="402" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="duplicateValues" dxfId="402" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="401" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="duplicateValues" dxfId="401" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="400" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="duplicateValues" dxfId="400" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="399" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3">
-    <cfRule type="duplicateValues" dxfId="399" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="398" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3">
-    <cfRule type="duplicateValues" dxfId="398" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="397" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="duplicateValues" dxfId="397" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="396" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="duplicateValues" dxfId="396" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="395" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="duplicateValues" dxfId="395" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="394" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="duplicateValues" dxfId="394" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="393" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="duplicateValues" dxfId="393" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="392" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="duplicateValues" dxfId="392" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="391" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="duplicateValues" dxfId="391" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="390" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="duplicateValues" dxfId="390" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="389" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="duplicateValues" dxfId="389" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="388" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="duplicateValues" dxfId="388" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="387" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="duplicateValues" dxfId="387" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="386" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="duplicateValues" dxfId="386" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="385" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="duplicateValues" dxfId="385" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="384" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="duplicateValues" dxfId="384" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="383" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="duplicateValues" dxfId="383" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="382" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="duplicateValues" dxfId="382" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="381" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="duplicateValues" dxfId="381" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="380" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="duplicateValues" dxfId="380" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="379" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="duplicateValues" dxfId="379" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="378" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="duplicateValues" dxfId="378" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="377" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="duplicateValues" dxfId="377" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="376" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="duplicateValues" dxfId="376" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="375" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="duplicateValues" dxfId="375" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="374" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="duplicateValues" dxfId="374" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="373" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="duplicateValues" dxfId="373" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="372" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="duplicateValues" dxfId="372" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="371" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="duplicateValues" dxfId="371" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="370" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3">
-    <cfRule type="duplicateValues" dxfId="370" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="369" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="duplicateValues" dxfId="369" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="368" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="duplicateValues" dxfId="368" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="367" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="duplicateValues" dxfId="367" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="366" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7">
-    <cfRule type="duplicateValues" dxfId="366" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="365" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8">
-    <cfRule type="duplicateValues" dxfId="365" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="364" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="duplicateValues" dxfId="364" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="363" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O10">
-    <cfRule type="duplicateValues" dxfId="363" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="362" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="duplicateValues" dxfId="362" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="361" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="duplicateValues" dxfId="361" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="360" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="duplicateValues" dxfId="360" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="359" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="duplicateValues" dxfId="359" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="358" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="duplicateValues" dxfId="358" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="357" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="duplicateValues" dxfId="357" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="356" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="duplicateValues" dxfId="356" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="355" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="duplicateValues" dxfId="355" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="354" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -11122,141 +12863,53 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="354" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="353" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="353" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="352" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="352" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="351" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="351" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="350" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="350" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="349" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="duplicateValues" dxfId="349" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="348" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="duplicateValues" dxfId="348" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="347" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="duplicateValues" dxfId="347" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="346" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="346" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="345" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="345" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="344" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="duplicateValues" dxfId="344" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="343" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="343" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="342" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="duplicateValues" dxfId="342" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="341" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="duplicateValues" dxfId="341" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="340" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="340" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="339" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="duplicateValues" dxfId="339" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="338" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="338" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="337" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="336" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="duplicateValues" dxfId="335" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="334" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="333" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="duplicateValues" dxfId="332" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="331" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
New Scenario for Manage Admins
</commit_message>
<xml_diff>
--- a/slingshot/TestData/InputData.xlsx
+++ b/slingshot/TestData/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15120" windowHeight="1920" tabRatio="871" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15120" windowHeight="1920" tabRatio="871" firstSheet="15" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Failure" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="234">
   <si>
     <t>Expected Messages</t>
   </si>
@@ -449,9 +449,6 @@
     <t>success_message</t>
   </si>
   <si>
-    <t>testkppodworks@gmail.com</t>
-  </si>
-  <si>
     <t>Manage_Train</t>
   </si>
   <si>
@@ -734,23 +731,20 @@
     <t>lastAfterPosting_date,lastAfterExpiry_date,postingBeforeExpiry_date,jobpostingBeforeLast_date,expiryAfterPosting_date,expiryAfterLast_date</t>
   </si>
   <si>
-    <t>bishnu.das@sakhatech.com</t>
-  </si>
-  <si>
-    <t>Password@123</t>
-  </si>
-  <si>
     <t>Aditya</t>
   </si>
   <si>
     <t>Yadav</t>
+  </si>
+  <si>
+    <t>aditya.yadav@sakhatech.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -934,8 +928,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="30">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1086,6 +1087,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -1296,7 +1303,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1323,9 +1330,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="26" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1382,6 +1386,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="28" fillId="30" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="28" fillId="30" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="57">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -8221,10 +8229,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="19"/>
+    <col min="1" max="1" width="21.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -8266,537 +8274,537 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.85546875" style="23"/>
-    <col min="5" max="5" width="21" style="23" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="23" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="23"/>
-    <col min="9" max="9" width="12" style="23" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" style="23"/>
-    <col min="12" max="12" width="32.28515625" style="25" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="23"/>
+    <col min="1" max="4" width="8.85546875" style="22"/>
+    <col min="5" max="5" width="21" style="22" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="22" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="22"/>
+    <col min="9" max="9" width="12" style="22" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" style="22"/>
+    <col min="12" max="12" width="32.28515625" style="24" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="24" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="26" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="26" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="26" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="K7" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L7" s="27" t="s">
+      <c r="L7" s="26" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="L8" s="26" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="26" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27" t="s">
+      <c r="H10" s="26"/>
+      <c r="I10" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L10" s="27" t="s">
+      <c r="L10" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K11" s="27" t="s">
+      <c r="K11" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="L11" s="26" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27" t="s">
+      <c r="I12" s="26"/>
+      <c r="J12" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L12" s="27" t="s">
+      <c r="L12" s="26" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K13" s="27" t="s">
+      <c r="K13" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L13" s="27" t="s">
+      <c r="L13" s="26" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I14" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27" t="s">
+      <c r="J14" s="26"/>
+      <c r="K14" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L14" s="27" t="s">
+      <c r="L14" s="26" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="K15" s="27" t="s">
+      <c r="K15" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L15" s="27" t="s">
+      <c r="L15" s="26" t="s">
         <v>100</v>
       </c>
     </row>
@@ -9454,34 +9462,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="29" t="s">
         <v>121</v>
       </c>
     </row>
@@ -9498,7 +9506,7 @@
       <c r="D2" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="33" t="s">
         <v>132</v>
       </c>
       <c r="F2" t="s">
@@ -9561,34 +9569,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="29" t="s">
         <v>121</v>
       </c>
     </row>
@@ -9602,7 +9610,7 @@
       <c r="C2" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="12" t="s">
@@ -9661,34 +9669,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="29" t="s">
         <v>121</v>
       </c>
     </row>
@@ -9702,7 +9710,7 @@
       <c r="C2" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="12" t="s">
@@ -9749,7 +9757,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9772,11 +9780,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>232</v>
+      <c r="A2" s="35" t="s">
+        <v>233</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -9804,10 +9812,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>134</v>
       </c>
     </row>
@@ -9826,52 +9834,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="7"/>
-    <col min="4" max="4" width="23.5703125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="13"/>
+    <col min="1" max="1" width="18" style="7" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="13" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="13" customWidth="1"/>
+    <col min="7" max="8" width="21.5703125" style="13" customWidth="1"/>
     <col min="9" max="9" width="16" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="13" customWidth="1"/>
     <col min="11" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="41" t="s">
         <v>105</v>
       </c>
     </row>
@@ -9879,12 +9888,12 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="9" t="s">
         <v>80</v>
       </c>
@@ -9903,16 +9912,16 @@
       <c r="C3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="9" t="s">
@@ -9935,14 +9944,14 @@
       <c r="C4" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="9" t="s">
@@ -9965,16 +9974,16 @@
       <c r="C5" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -9997,16 +10006,16 @@
       <c r="C6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -10029,14 +10038,14 @@
       <c r="C7" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="9" t="s">
@@ -10059,16 +10068,16 @@
       <c r="C8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="17"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="9" t="s">
         <v>80</v>
       </c>
@@ -10090,12 +10099,12 @@
         <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="12" t="s">
@@ -10107,7 +10116,7 @@
       <c r="I9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="16" t="s">
         <v>92</v>
       </c>
     </row>
@@ -10121,16 +10130,16 @@
       <c r="C10" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>132</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="H10" s="9" t="s">
@@ -10139,7 +10148,7 @@
       <c r="I10" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="16" t="s">
         <v>127</v>
       </c>
     </row>
@@ -10288,9 +10297,6 @@
   <conditionalFormatting sqref="G10">
     <cfRule type="duplicateValues" dxfId="11" priority="48"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="duplicateValues" dxfId="10" priority="49"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A2:B2">
     <cfRule type="duplicateValues" dxfId="9" priority="50"/>
   </conditionalFormatting>
@@ -10307,7 +10313,7 @@
     <cfRule type="duplicateValues" dxfId="5" priority="54"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10438,7 +10444,7 @@
       <c r="I2" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>136</v>
       </c>
     </row>
@@ -10481,21 +10487,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -10594,7 +10600,7 @@
       <c r="C2" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>84</v>
       </c>
       <c r="E2" s="12" t="s">
@@ -10618,15 +10624,15 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>84</v>
       </c>
       <c r="E3" s="12" t="s">
@@ -10658,7 +10664,7 @@
       <c r="C4" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>84</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -10729,99 +10735,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="37" t="s">
+      <c r="K1" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="L1" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="M1" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="N1" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="O1" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="P1" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="Q1" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="R1" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="S1" s="36" t="s">
         <v>158</v>
-      </c>
-      <c r="S1" s="37" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="90" x14ac:dyDescent="0.25">
-      <c r="S2" s="38" t="s">
-        <v>161</v>
+      <c r="S2" s="37" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="120" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="G3" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="I3" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H3" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L3" s="2">
         <v>42840</v>
@@ -10829,55 +10835,55 @@
       <c r="M3" s="2">
         <v>42832</v>
       </c>
-      <c r="N3" s="33">
+      <c r="N3" s="32">
         <v>42885</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P3" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="Q3" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R3" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="D4" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="G4" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="I4" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H4" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L4" s="2">
         <v>42840</v>
@@ -10885,56 +10891,56 @@
       <c r="M4" s="2">
         <v>42832</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="32">
         <v>42885</v>
       </c>
       <c r="O4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P4" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P4" s="38" t="s">
+      <c r="Q4" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R4" s="39" t="s">
+      <c r="S4" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33" t="s">
+      <c r="C5" s="32"/>
+      <c r="D5" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="F5" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="G5" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H5" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="I5" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H5" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L5" s="2">
         <v>42840</v>
@@ -10942,56 +10948,56 @@
       <c r="M5" s="2">
         <v>42832</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5" s="32">
         <v>42885</v>
       </c>
       <c r="O5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P5" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P5" s="38" t="s">
+      <c r="Q5" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R5" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S5" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B6" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="G6" s="33" t="s">
+      <c r="I6" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H6" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L6" s="2">
         <v>42840</v>
@@ -10999,56 +11005,56 @@
       <c r="M6" s="2">
         <v>42832</v>
       </c>
-      <c r="N6" s="33">
+      <c r="N6" s="32">
         <v>42885</v>
       </c>
       <c r="O6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P6" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P6" s="38" t="s">
+      <c r="Q6" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R6" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S6" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H7" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="I7" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H7" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L7" s="2">
         <v>42840</v>
@@ -11056,56 +11062,56 @@
       <c r="M7" s="2">
         <v>42832</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="32">
         <v>42885</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P7" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P7" s="38" t="s">
+      <c r="Q7" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R7" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S7" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H8" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L8" s="2">
         <v>42840</v>
@@ -11113,56 +11119,56 @@
       <c r="M8" s="2">
         <v>42832</v>
       </c>
-      <c r="N8" s="33">
+      <c r="N8" s="32">
         <v>42885</v>
       </c>
       <c r="O8" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P8" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P8" s="38" t="s">
+      <c r="Q8" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R8" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S8" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="E9" s="33" t="s">
+      <c r="F9" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="G9" s="32"/>
+      <c r="H9" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33" t="s">
-        <v>167</v>
-      </c>
       <c r="I9" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L9" s="2">
         <v>42840</v>
@@ -11170,56 +11176,56 @@
       <c r="M9" s="2">
         <v>42832</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="32">
         <v>42885</v>
       </c>
       <c r="O9" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P9" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P9" s="38" t="s">
+      <c r="Q9" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="R9" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R9" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S9" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="E10" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F10" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L10" s="2">
         <v>42840</v>
@@ -11227,55 +11233,55 @@
       <c r="M10" s="2">
         <v>42832</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="32">
         <v>42885</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P10" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P10" s="38" t="s">
+      <c r="Q10" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="R10" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R10" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S10" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>199</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="E11" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="G11" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H11" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G11" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>167</v>
-      </c>
       <c r="J11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L11" s="2">
         <v>42840</v>
@@ -11283,55 +11289,55 @@
       <c r="M11" s="2">
         <v>42832</v>
       </c>
-      <c r="N11" s="33">
+      <c r="N11" s="32">
         <v>42885</v>
       </c>
       <c r="O11" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P11" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P11" s="38" t="s">
+      <c r="Q11" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="R11" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R11" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S11" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="E12" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="G12" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="I12" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H12" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="K12" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L12" s="2">
         <v>42840</v>
@@ -11339,55 +11345,55 @@
       <c r="M12" s="2">
         <v>42832</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="32">
         <v>42885</v>
       </c>
       <c r="O12" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P12" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P12" s="38" t="s">
+      <c r="Q12" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="R12" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R12" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S12" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>214</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="E13" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F13" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="G13" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H13" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="I13" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H13" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="L13" s="2">
         <v>42840</v>
@@ -11395,170 +11401,170 @@
       <c r="M13" s="2">
         <v>42832</v>
       </c>
-      <c r="N13" s="33">
+      <c r="N13" s="32">
         <v>42885</v>
       </c>
       <c r="O13" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P13" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P13" s="38" t="s">
+      <c r="Q13" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="R13" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R13" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S13" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="E14" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F14" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="G14" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H14" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="I14" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H14" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="M14" s="2">
         <v>42832</v>
       </c>
-      <c r="N14" s="33">
+      <c r="N14" s="32">
         <v>42885</v>
       </c>
       <c r="O14" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P14" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P14" s="38" t="s">
+      <c r="Q14" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="R14" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R14" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S14" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="E15" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F15" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="G15" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H15" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="I15" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H15" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L15" s="2">
         <v>42840</v>
       </c>
-      <c r="N15" s="33">
+      <c r="N15" s="32">
         <v>42885</v>
       </c>
       <c r="O15" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P15" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P15" s="38" t="s">
+      <c r="Q15" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="R15" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R15" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S15" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>204</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="E16" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F16" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="G16" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H16" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G16" s="33" t="s">
+      <c r="I16" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H16" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L16" s="2">
         <v>42840</v>
@@ -11566,56 +11572,56 @@
       <c r="M16" s="2">
         <v>42832</v>
       </c>
-      <c r="N16" s="33"/>
+      <c r="N16" s="32"/>
       <c r="O16" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P16" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P16" s="38" t="s">
+      <c r="Q16" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="R16" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R16" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S16" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>205</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>222</v>
-      </c>
-      <c r="E17" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="G17" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H17" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G17" s="33" t="s">
+      <c r="I17" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H17" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L17" s="2">
         <v>42840</v>
@@ -11623,55 +11629,55 @@
       <c r="M17" s="2">
         <v>42832</v>
       </c>
-      <c r="N17" s="33">
+      <c r="N17" s="32">
         <v>42885</v>
       </c>
-      <c r="P17" s="38" t="s">
+      <c r="P17" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q17" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="R17" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R17" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S17" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>223</v>
-      </c>
-      <c r="E18" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F18" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="G18" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H18" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="I18" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H18" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L18" s="2">
         <v>42840</v>
@@ -11679,56 +11685,56 @@
       <c r="M18" s="2">
         <v>42832</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N18" s="32">
         <v>42885</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="P18" s="38"/>
+        <v>171</v>
+      </c>
+      <c r="P18" s="37"/>
       <c r="Q18" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="R18" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R18" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S18" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>207</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="E19" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F19" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="G19" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H19" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="I19" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H19" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L19" s="2">
         <v>42840</v>
@@ -11736,56 +11742,56 @@
       <c r="M19" s="2">
         <v>42832</v>
       </c>
-      <c r="N19" s="33">
+      <c r="N19" s="32">
         <v>42885</v>
       </c>
       <c r="O19" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P19" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P19" s="38" t="s">
+      <c r="Q19" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q19" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="R19" s="39"/>
+      <c r="R19" s="38"/>
       <c r="S19" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="E20" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="G20" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="I20" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H20" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L20" s="2">
         <v>42840</v>
@@ -11793,58 +11799,58 @@
       <c r="M20" s="2">
         <v>42832</v>
       </c>
-      <c r="N20" s="33">
+      <c r="N20" s="32">
         <v>42885</v>
       </c>
       <c r="O20" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P20" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P20" s="38" t="s">
+      <c r="Q20" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="R20" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R20" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S20" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="E21" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="H21" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="F21" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="G21" s="33" t="s">
+      <c r="I21" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="H21" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L21" s="2">
         <v>42840</v>
@@ -11852,58 +11858,58 @@
       <c r="M21" s="2">
         <v>42832</v>
       </c>
-      <c r="N21" s="33">
+      <c r="N21" s="32">
         <v>42885</v>
       </c>
       <c r="O21" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P21" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P21" s="38" t="s">
+      <c r="Q21" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="R21" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R21" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S21" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="E22" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F22" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="G22" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G22" s="33" t="s">
+      <c r="H22" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="I22" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L22" s="2">
         <v>42840</v>
@@ -11911,58 +11917,58 @@
       <c r="M22" s="2">
         <v>42832</v>
       </c>
-      <c r="N22" s="33">
+      <c r="N22" s="32">
         <v>42885</v>
       </c>
       <c r="O22" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P22" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P22" s="38" t="s">
+      <c r="Q22" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="R22" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R22" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S22" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="D23" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="E23" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F23" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="G23" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="H23" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="I23" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L23" s="2">
         <v>42834</v>
@@ -11974,54 +11980,54 @@
         <v>42852</v>
       </c>
       <c r="O23" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P23" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P23" s="38" t="s">
+      <c r="Q23" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="R23" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R23" s="39" t="s">
-        <v>175</v>
-      </c>
       <c r="S23" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="E24" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="G24" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G24" s="33" t="s">
+      <c r="H24" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="I24" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L24" s="2">
         <v>42846</v>
@@ -12033,54 +12039,54 @@
         <v>42836</v>
       </c>
       <c r="O24" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P24" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P24" s="38" t="s">
+      <c r="Q24" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="R24" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R24" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="S24" s="38" t="s">
-        <v>230</v>
+      <c r="S24" s="37" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="E25" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="G25" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="H25" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="I25" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="L25" s="2">
         <v>42875</v>
@@ -12092,19 +12098,19 @@
         <v>42836</v>
       </c>
       <c r="O25" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P25" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P25" s="38" t="s">
+      <c r="Q25" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="Q25" s="2" t="s">
+      <c r="R25" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="R25" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="S25" s="38" t="s">
-        <v>231</v>
+      <c r="S25" s="37" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -13202,7 +13208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -13214,16 +13220,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code for User Edit Profile
</commit_message>
<xml_diff>
--- a/slingshot/TestData/InputData.xlsx
+++ b/slingshot/TestData/InputData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15120" windowHeight="1920" tabRatio="871" firstSheet="16" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15120" windowHeight="1920" tabRatio="871" firstSheet="17" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Failure" sheetId="10" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="AddSubAdmin_Success" sheetId="25" r:id="rId19"/>
     <sheet name="AnotherAdminErrorMsg_Success" sheetId="22" r:id="rId20"/>
     <sheet name="AddAdmin_Failure" sheetId="19" r:id="rId21"/>
-    <sheet name="TestCal_Success" sheetId="41" r:id="rId22"/>
+    <sheet name="UserBaisicInfo_Failure" sheetId="41" r:id="rId22"/>
     <sheet name="LoginAsRemovedAdmin_Success" sheetId="20" r:id="rId23"/>
     <sheet name="AddAnotherAdmin_Success" sheetId="21" r:id="rId24"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="248">
   <si>
     <t>Expected Messages</t>
   </si>
@@ -741,16 +741,46 @@
     <t>aditya.yadav@sakhatech.com</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Password@123</t>
   </si>
   <si>
     <t>bishnu29das@gmail.com</t>
   </si>
   <si>
-    <t>2003-05-03</t>
+    <t xml:space="preserve">First Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender </t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Address Line 1</t>
+  </si>
+  <si>
+    <t>Address Line 2</t>
+  </si>
+  <si>
+    <t>Address Line 3</t>
+  </si>
+  <si>
+    <t>Pin Code</t>
+  </si>
+  <si>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>fname_req,age_req,gender_req,dob_req,maritalstatus_req,addline1_req,city_req,pin_req,emailid_req,mobile_req</t>
   </si>
 </sst>
 </file>
@@ -9792,10 +9822,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -10330,30 +10360,82 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="89.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" s="36" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>237</v>
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="O2" s="37" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>